<commit_message>
Corrección del seleniuro por el selenuro
</commit_message>
<xml_diff>
--- a/client/public/Hojas de Calculo/nometales.xlsx
+++ b/client/public/Hojas de Calculo/nometales.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">Seleniuro</t>
+    <t xml:space="preserve">Selenuro</t>
   </si>
   <si>
     <t xml:space="preserve">Se</t>
@@ -211,10 +211,10 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:B13"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
   </cols>
@@ -326,10 +326,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>